<commit_message>
modify files related to home and searchListing Page and added new files for HotelDetail Review Page
</commit_message>
<xml_diff>
--- a/src/test/resouces/SearchCriteria.xlsx
+++ b/src/test/resouces/SearchCriteria.xlsx
@@ -11,16 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Checkin</t>
-  </si>
-  <si>
-    <t>CheckOut</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>RoomCount</t>
   </si>
@@ -47,15 +38,6 @@
   </si>
   <si>
     <t>UserRating</t>
-  </si>
-  <si>
-    <t>Goa</t>
-  </si>
-  <si>
-    <t>Sun, 14 March 2021</t>
-  </si>
-  <si>
-    <t>Mon, 15 March 2021</t>
   </si>
   <si>
     <t>1</t>
@@ -89,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -106,11 +88,6 @@
       <color indexed="9"/>
       <name val="Helvetica Neue"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="9"/>
-      <name val="Helvetica Neue Medium"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -121,12 +98,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="15"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -190,7 +167,7 @@
         <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -199,34 +176,19 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
         <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -235,7 +197,7 @@
         <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -247,10 +209,10 @@
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -259,43 +221,28 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -307,7 +254,7 @@
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -319,10 +266,10 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -331,28 +278,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -365,7 +297,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -381,7 +313,7 @@
     <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -390,43 +322,34 @@
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -450,7 +373,6 @@
       <rgbColor rgb="ffadadad"/>
       <rgbColor rgb="ffd6d6d6"/>
       <rgbColor rgb="ff89847f"/>
-      <rgbColor rgb="ffa6a29f"/>
       <rgbColor rgb="ffe3e3e3"/>
       <rgbColor rgb="fff4f9f8"/>
     </indexedColors>
@@ -1511,20 +1433,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
+      <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.8984" style="1" customWidth="1"/>
-    <col min="4" max="11" width="16.3516" style="1" customWidth="1"/>
-    <col min="12" max="12" width="26.3594" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.3594" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.55" customHeight="1">
@@ -1552,338 +1471,260 @@
       <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" t="s" s="4">
         <v>8</v>
-      </c>
-      <c r="J1" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s" s="4">
-        <v>11</v>
       </c>
     </row>
     <row r="2" ht="20.3" customHeight="1">
       <c r="A2" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="B2" t="s" s="6">
+      <c r="G2" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="C2" t="s" s="7">
+      <c r="H2" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D2" t="s" s="7">
+      <c r="I2" t="s" s="7">
         <v>15</v>
       </c>
-      <c r="E2" t="s" s="7">
+    </row>
+    <row r="3" ht="19.95" customHeight="1">
+      <c r="A3" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="F2" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s" s="7">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s" s="7">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s" s="7">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s" s="7">
-        <v>19</v>
-      </c>
-      <c r="K2" t="s" s="7">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s" s="8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" ht="19.95" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
     </row>
     <row r="4" ht="19.95" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" ht="19.95" customHeight="1">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="10"/>
     </row>
     <row r="6" ht="19.95" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="16"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" ht="19.95" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="10"/>
     </row>
     <row r="8" ht="19.95" customHeight="1">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="16"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" ht="19.95" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" ht="19.95" customHeight="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="16"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" ht="19.95" customHeight="1">
-      <c r="A11" s="13"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="12"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" ht="19.95" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="16"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" ht="19.95" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
     </row>
     <row r="14" ht="19.95" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="16"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" ht="19.95" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="12"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
     </row>
     <row r="16" ht="19.95" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="16"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" ht="19.95" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="12"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
     </row>
     <row r="18" ht="19.95" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="16"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
     </row>
     <row r="19" ht="19.95" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" ht="19.95" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="16"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
     </row>
     <row r="21" ht="19.95" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="12"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
     </row>
     <row r="22" ht="20.2" customHeight="1">
-      <c r="A22" s="17"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="20"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
change is excel file and pom file
</commit_message>
<xml_diff>
--- a/src/test/resouces/SearchCriteria.xlsx
+++ b/src/test/resouces/SearchCriteria.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>RoomCount</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>4 &amp; above (Very Good)</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>END</t>
@@ -297,7 +300,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -325,25 +328,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1433,7 +1424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="A2" xSplit="0" ySplit="1" activePane="bottomLeft" state="frozen"/>
@@ -1506,19 +1497,35 @@
     </row>
     <row r="3" ht="19.95" customHeight="1">
       <c r="A3" t="s" s="8">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="9">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="9">
+        <v>11</v>
+      </c>
       <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10"/>
+      <c r="G3" t="s" s="9">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s" s="9">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s" s="10">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" ht="19.95" customHeight="1">
-      <c r="A4" s="11"/>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="11">
+        <v>17</v>
+      </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -1528,204 +1535,6 @@
       <c r="H4" s="12"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" ht="19.95" customHeight="1">
-      <c r="A5" s="14"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10"/>
-    </row>
-    <row r="6" ht="19.95" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" ht="19.95" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="10"/>
-    </row>
-    <row r="8" ht="19.95" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" ht="19.95" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="10"/>
-    </row>
-    <row r="10" ht="19.95" customHeight="1">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="13"/>
-    </row>
-    <row r="11" ht="19.95" customHeight="1">
-      <c r="A11" s="14"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" ht="19.95" customHeight="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="13"/>
-    </row>
-    <row r="13" ht="19.95" customHeight="1">
-      <c r="A13" s="14"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="10"/>
-    </row>
-    <row r="14" ht="19.95" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-    </row>
-    <row r="15" ht="19.95" customHeight="1">
-      <c r="A15" s="14"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-    </row>
-    <row r="16" ht="19.95" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="13"/>
-    </row>
-    <row r="17" ht="19.95" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" ht="19.95" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="13"/>
-    </row>
-    <row r="19" ht="19.95" customHeight="1">
-      <c r="A19" s="14"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" ht="19.95" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13"/>
-    </row>
-    <row r="21" ht="19.95" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" ht="20.2" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-    </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>